<commit_message>
added partitioned value axis to PSII trends bar chart
</commit_message>
<xml_diff>
--- a/test/pesticides.xlsx
+++ b/test/pesticides.xlsx
@@ -187,13 +187,13 @@
   </sheetPr>
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A18" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="J58" activeCellId="0" pane="topLeft" sqref="J58"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.878431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9803921568627"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="1">
@@ -1016,25 +1016,25 @@
         <v>17</v>
       </c>
       <c r="D32" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E32" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>3</v>
+        <v>100</v>
       </c>
       <c r="H32" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I32" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J32" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="33">
@@ -1684,25 +1684,25 @@
         <v>17</v>
       </c>
       <c r="D57" s="0" t="n">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E57" s="0" t="n">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="F57" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G57" s="0" t="n">
-        <v>3</v>
+        <v>460</v>
       </c>
       <c r="H57" s="0" t="n">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="I57" s="0" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J57" s="0" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="58">
@@ -1864,7 +1864,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1889,7 +1889,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.6941176470588"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>